<commit_message>
alterando o nome da coluna de valores
</commit_message>
<xml_diff>
--- a/catalogo.xlsx
+++ b/catalogo.xlsx
@@ -1,37 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29816"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gustavo.maciel\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFAB7494-E1F1-48D6-9692-91AA32B3DFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{03957708-364E-4929-8180-F1BB17ABC805}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Planilha1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -56,7 +34,7 @@
     <t>Descrição Curta GSC</t>
   </si>
   <si>
-    <t>Fabrica</t>
+    <t>Preço</t>
   </si>
   <si>
     <t>Descrição Longa  GSC</t>
@@ -878,11 +856,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -893,10 +869,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -908,12 +889,33 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFffff00"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFc6c6c6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFc6c6c6"/>
+      </bottom>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -925,39 +927,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="15">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -968,10 +990,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -998,116 +1020,82 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1119,166 +1107,191 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1FE0445-D577-4384-9D9B-663C3FA8706E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="73.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="10" width="25.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="8.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="25.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="7.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="33.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="14" width="10.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="73.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="26.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1294,7 +1307,7 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -1310,1991 +1323,1991 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>303024</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="7">
         <v>7896004742076</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="9">
         <v>225.36</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="6">
         <v>100804</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="7">
         <v>7896015520380</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="9">
         <v>163.9</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <v>401958</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="7">
         <v>7891010256708</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="9">
         <v>36.19</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <v>101545</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="7">
         <v>7891142156020</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="9">
         <v>67.81</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <v>110681</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="7">
         <v>7896026306720</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="9">
         <v>384.83</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <v>110999</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="7">
         <v>7896658027123</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="9">
         <v>72.58</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <v>715095</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="7">
         <v>4005900521897</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="9">
         <v>31.6</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <v>401214</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="7">
         <v>7896015520533</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="9">
         <v>74.38</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="6">
         <v>303621</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="7">
         <v>7897595631770</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="9">
         <v>27.8</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="6">
         <v>306760</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="7">
         <v>7897595637161</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="9">
         <v>152.1</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <v>724065</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="7">
         <v>7908785490227</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="9">
         <v>76.91</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="6">
         <v>109782</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="7">
         <v>7897322714257</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="9">
         <v>32.44</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="6">
         <v>112060</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="7">
         <v>7896112402749</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="9">
         <v>54.79</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="6">
         <v>720948</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="7">
         <v>7896009498596</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="9">
         <v>26.37</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="6">
         <v>105680</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="7">
         <v>7896112405870</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="9">
         <v>207.26</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" t="s">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="6">
         <v>100299</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="7">
         <v>7896637018029</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="9">
         <v>14</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18" t="s">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="6">
         <v>107754</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="7">
         <v>7891317192792</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="9">
         <v>86.39</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" t="s">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="6">
         <v>707772</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="7">
         <v>7891010601188</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G19" s="7">
-        <v>18.059999999999999</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="G19" s="9">
+        <v>18.06</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" t="s">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="6">
         <v>721953</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="7">
         <v>7891142982759</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="9">
         <v>85.04</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" t="s">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="6">
         <v>721858</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="7">
         <v>7896012880036</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="9">
         <v>200.09</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22" t="s">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="6">
         <v>101126</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="7">
         <v>7896422515085</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="9">
         <v>88.49</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" t="s">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="6">
         <v>112304</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="7">
         <v>7896094925137</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="9">
         <v>69.75</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" t="s">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="6">
         <v>111711</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="7">
         <v>7899420507410</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="9">
         <v>44.05</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" t="s">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="6">
         <v>302311</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="7">
         <v>7891317434342</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="9">
         <v>216.59</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" t="s">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="6">
         <v>723404</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="7">
         <v>7891317038717</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="9">
         <v>114.55</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
-      <c r="A27" t="s">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="A27" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="6">
         <v>102816</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="7">
         <v>7896026303088</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="G27" s="7">
-        <v>156.13999999999999</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="G27" s="9">
+        <v>156.14</v>
+      </c>
+      <c r="H27" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="A28" t="s">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+      <c r="A28" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="6">
         <v>400101</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="7">
         <v>7891317002589</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="G28" s="7">
-        <v>17.260000000000002</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="G28" s="9">
+        <v>17.26</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
-      <c r="A29" t="s">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+      <c r="A29" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="6">
         <v>115403</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="7">
         <v>7896112409823</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="9">
         <v>59</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
-      <c r="A30" t="s">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+      <c r="A30" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="6">
         <v>710673</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="7">
         <v>7891010518844</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="9">
         <v>22.68</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
-      <c r="A31" t="s">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+      <c r="A31" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="6">
         <v>402700</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="7">
         <v>7898928257025</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="9">
         <v>101.64</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
-      <c r="A32" t="s">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+      <c r="A32" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="6">
         <v>111998</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="7">
         <v>7898029550803</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="9">
         <v>68.33</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
-      <c r="A33" t="s">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+      <c r="A33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="6">
         <v>102447</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="7">
         <v>7894916500425</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="G33" s="7">
-        <v>36.090000000000003</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="G33" s="9">
+        <v>36.09</v>
+      </c>
+      <c r="H33" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
-      <c r="A34" t="s">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+      <c r="A34" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="6">
         <v>309070</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="7">
         <v>7896004820910</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="9">
         <v>86.1</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J34" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35" t="s">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+      <c r="A35" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="6">
         <v>719607</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="7">
         <v>4005900921567</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="9">
         <v>20.61</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J35" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
-      <c r="A36" t="s">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+      <c r="A36" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="6">
         <v>405920</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="7">
         <v>7896026173247</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="9">
         <v>27.8</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J36" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37" t="s">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+      <c r="A37" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="6">
         <v>103451</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="7">
         <v>7896006219095</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="9">
         <v>42.88</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J37" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
-      <c r="A38" t="s">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+      <c r="A38" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38" s="6">
         <v>723668</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="7">
         <v>7908950000008</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G38" s="9">
         <v>94.34</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
-      <c r="A39" t="s">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+      <c r="A39" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D39" s="6">
         <v>115205</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="7">
         <v>7891317038656</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="G39" s="7">
+      <c r="G39" s="9">
         <v>72.25</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J39" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
-      <c r="A40" t="s">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+      <c r="A40" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D40" s="6">
         <v>723247</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="7">
         <v>7891033718641</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="G40" s="7">
-        <v>38.770000000000003</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="G40" s="9">
+        <v>38.77</v>
+      </c>
+      <c r="H40" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
-      <c r="A41" t="s">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+      <c r="A41" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D41" s="6">
         <v>714549</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="7">
         <v>7896015590932</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="G41" s="7">
+      <c r="G41" s="9">
         <v>24.61</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="A42" t="s">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+      <c r="A42" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="6">
         <v>400632</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="7">
         <v>7896004817774</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="G42" s="7">
+      <c r="G42" s="9">
         <v>308.24</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H42" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J42" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
-      <c r="A43" t="s">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+      <c r="A43" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43" s="6">
         <v>105278</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="7">
         <v>7896658017643</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="G43" s="7">
+      <c r="G43" s="9">
         <v>117.18</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H43" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J43" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
-      <c r="A44" t="s">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+      <c r="A44" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D44" s="6">
         <v>112767</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="7">
         <v>7891317010386</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="G44" s="7">
+      <c r="G44" s="9">
         <v>53.04</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H44" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J44" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
-      <c r="A45" t="s">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+      <c r="A45" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D45" s="5">
+      <c r="D45" s="6">
         <v>400928</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="7">
         <v>7896094922129</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="G45" s="7">
+      <c r="G45" s="9">
         <v>20.89</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H45" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="J45" t="s">
+      <c r="J45" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
-      <c r="A46" t="s">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+      <c r="A46" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D46" s="5">
+      <c r="D46" s="6">
         <v>708942</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="7">
         <v>7897322714288</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="G46" s="7">
+      <c r="G46" s="9">
         <v>35.79</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I46" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J46" s="5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
-      <c r="A47" t="s">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+      <c r="A47" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D47" s="6">
         <v>401067</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="7">
         <v>7896512904126</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="G47" s="7">
+      <c r="G47" s="9">
         <v>12.03</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J47" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
-      <c r="A48" t="s">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+      <c r="A48" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="5">
+      <c r="D48" s="6">
         <v>112608</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="7">
         <v>7896658038556</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="G48" s="7">
+      <c r="G48" s="9">
         <v>174</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H48" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I48" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J48" s="5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
-      <c r="A49" t="s">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+      <c r="A49" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D49" s="5">
+      <c r="D49" s="6">
         <v>104396</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="7">
         <v>7891317472061</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="G49" s="7">
+      <c r="G49" s="9">
         <v>69.62</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I49" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" s="5" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
-      <c r="A50" t="s">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+      <c r="A50" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D50" s="5">
+      <c r="D50" s="6">
         <v>102321</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="7">
         <v>7896637025102</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="F50" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="G50" s="7">
+      <c r="G50" s="9">
         <v>27.08</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H50" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I50" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="5" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
-      <c r="A51" t="s">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+      <c r="A51" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="D51" s="5">
+      <c r="D51" s="6">
         <v>723799</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E51" s="7">
         <v>7897129305351</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F51" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="G51" s="7">
+      <c r="G51" s="9">
         <v>54.38</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I51" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J51" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
-      <c r="A52" t="s">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+      <c r="A52" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D52" s="5">
+      <c r="D52" s="6">
         <v>400888</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52" s="7">
         <v>7891010256425</v>
       </c>
-      <c r="F52" s="5" t="s">
+      <c r="F52" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="G52" s="7">
+      <c r="G52" s="9">
         <v>46.15</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H52" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I52" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="J52" t="s">
+      <c r="J52" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
-      <c r="A53" t="s">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+      <c r="A53" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="D53" s="5">
+      <c r="D53" s="6">
         <v>306862</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53" s="7">
         <v>7896658036347</v>
       </c>
-      <c r="F53" s="5" t="s">
+      <c r="F53" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="G53" s="7">
+      <c r="G53" s="9">
         <v>64.45</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H53" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I53" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J53" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
-      <c r="A54" t="s">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+      <c r="A54" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D54" s="5">
+      <c r="D54" s="6">
         <v>303610</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54" s="7">
         <v>7897595630605</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F54" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="G54" s="7">
+      <c r="G54" s="9">
         <v>45.82</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H54" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I54" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J54" s="5" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
-      <c r="A55" t="s">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+      <c r="A55" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="D55" s="5">
+      <c r="D55" s="6">
         <v>304063</v>
       </c>
-      <c r="E55" s="6">
+      <c r="E55" s="7">
         <v>7896181925224</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="F55" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="G55" s="7">
+      <c r="G55" s="9">
         <v>75.94</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H55" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I55" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J55" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
-      <c r="A56" t="s">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+      <c r="A56" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D56" s="5">
+      <c r="D56" s="6">
         <v>400930</v>
       </c>
-      <c r="E56" s="6">
+      <c r="E56" s="7">
         <v>7896094921979</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="G56" s="7">
+      <c r="G56" s="9">
         <v>27.67</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H56" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="J56" t="s">
+      <c r="J56" s="5" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
-      <c r="A57" t="s">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+      <c r="A57" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="D57" s="5">
+      <c r="D57" s="6">
         <v>710570</v>
       </c>
-      <c r="E57" s="6">
+      <c r="E57" s="7">
         <v>7896658029509</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="F57" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="G57" s="7">
+      <c r="G57" s="9">
         <v>89.44</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H57" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I57" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J57" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
-      <c r="A58" t="s">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+      <c r="A58" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D58" s="5">
+      <c r="D58" s="6">
         <v>723793</v>
       </c>
-      <c r="E58" s="6">
+      <c r="E58" s="7">
         <v>7891142982643</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="F58" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="G58" s="7">
+      <c r="G58" s="9">
         <v>182.42</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H58" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I58" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J58" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
-      <c r="A59" t="s">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+      <c r="A59" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="D59" s="5">
+      <c r="D59" s="6">
         <v>102461</v>
       </c>
-      <c r="E59" s="6">
+      <c r="E59" s="7">
         <v>7896206402181</v>
       </c>
-      <c r="F59" s="5" t="s">
+      <c r="F59" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="G59" s="7">
+      <c r="G59" s="9">
         <v>155.87</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H59" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I59" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J59" s="5" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
-      <c r="A60" t="s">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+      <c r="A60" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="D60" s="5">
+      <c r="D60" s="6">
         <v>103134</v>
       </c>
-      <c r="E60" s="6">
+      <c r="E60" s="7">
         <v>7891721012969</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="F60" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="G60" s="7">
+      <c r="G60" s="9">
         <v>23.42</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H60" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I60" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J60" t="s">
+      <c r="J60" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
-      <c r="A61" t="s">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+      <c r="A61" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D61" s="5">
+      <c r="D61" s="6">
         <v>112162</v>
       </c>
-      <c r="E61" s="6">
+      <c r="E61" s="7">
         <v>7896637032803</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="F61" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="G61" s="7">
+      <c r="G61" s="9">
         <v>85.57</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H61" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I61" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="J61" t="s">
+      <c r="J61" s="5" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
-      <c r="A62" t="s">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+      <c r="A62" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D62" s="5">
+      <c r="D62" s="6">
         <v>719710</v>
       </c>
-      <c r="E62" s="6">
+      <c r="E62" s="7">
         <v>4005900633309</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F62" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="G62" s="7">
+      <c r="G62" s="9">
         <v>13.75</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H62" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="I62" t="s">
+      <c r="I62" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J62" t="s">
+      <c r="J62" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
-      <c r="A63" t="s">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+      <c r="A63" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="D63" s="5">
+      <c r="D63" s="6">
         <v>723326</v>
       </c>
-      <c r="E63" s="6">
+      <c r="E63" s="7">
         <v>7908785461753</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="F63" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="G63" s="7">
+      <c r="G63" s="9">
         <v>11.63</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H63" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I63" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J63" t="s">
+      <c r="J63" s="5" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>